<commit_message>
-fixed output styles for repeat-until and section. Hopefully I get it right this time!
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90A220E-0806-CF40-9ED1-DBE6ED40E348}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC04BC5A-D343-0F49-8681-CDD73BD31B0D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="-20560" windowWidth="33600" windowHeight="20560" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="25160" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="895">
   <si>
     <t>description</t>
   </si>
@@ -2810,6 +2810,45 @@
   </si>
   <si>
     <t>check command name</t>
+  </si>
+  <si>
+    <t>simple section</t>
+  </si>
+  <si>
+    <t>First section of this simple section</t>
+  </si>
+  <si>
+    <t>counter1</t>
+  </si>
+  <si>
+    <t>Still in repeat-until loop, counter1=${counter1}</t>
+  </si>
+  <si>
+    <t>Last statement of this simple section</t>
+  </si>
+  <si>
+    <t>in-section loop starts</t>
+  </si>
+  <si>
+    <t>check for termination</t>
+  </si>
+  <si>
+    <t>… do task</t>
+  </si>
+  <si>
+    <t>get ready for next loop</t>
+  </si>
+  <si>
+    <t>out of loop, out of section</t>
+  </si>
+  <si>
+    <t>simple section starts</t>
+  </si>
+  <si>
+    <t>${counter1}</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -3353,6 +3392,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3403,10 +3446,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="32">
@@ -5640,12 +5679,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -5663,20 +5702,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -5686,10 +5725,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -6098,12 +6137,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="51" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -6121,20 +6160,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>840</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -6144,10 +6183,10 @@
       </c>
       <c r="J2" s="30"/>
       <c r="K2" s="31"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="71"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="72"/>
     </row>
     <row r="3" spans="1:15" s="51" customFormat="1" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
@@ -7247,12 +7286,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -7270,18 +7309,18 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -7291,10 +7330,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -7545,12 +7584,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -7568,20 +7607,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>406</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -7591,10 +7630,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -8016,12 +8055,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -8039,20 +8078,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -8062,10 +8101,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -10592,12 +10631,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -10615,20 +10654,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -10638,10 +10677,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -10966,12 +11005,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -10989,20 +11028,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -11012,10 +11051,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -11665,12 +11704,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -11688,20 +11727,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -11711,10 +11750,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -12616,12 +12655,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -12639,20 +12678,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -12662,10 +12701,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -13799,12 +13838,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -13822,20 +13861,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>406</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -13845,10 +13884,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -14440,12 +14479,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -14463,20 +14502,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -14486,10 +14525,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -25959,11 +25998,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25971,7 +26010,7 @@
     <col min="1" max="1" width="13.5" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="22" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.6640625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="25.6640625" style="9" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="23.1640625" style="9" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="36" style="25" customWidth="1" collapsed="1"/>
@@ -25984,12 +26023,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -26007,20 +26046,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -26030,10 +26069,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -26234,7 +26273,7 @@
     </row>
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="57" t="s">
         <v>881</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -26518,6 +26557,130 @@
       </c>
       <c r="E23" s="9" t="s">
         <v>872</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>882</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>892</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
+        <v>889</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>887</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="8" t="s">
+        <v>888</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>893</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="8" t="s">
+        <v>889</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="8" t="s">
+        <v>890</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+      <c r="B31" s="8" t="s">
+        <v>891</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>886</v>
       </c>
     </row>
   </sheetData>
@@ -26539,7 +26702,7 @@
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1048576" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>target</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
- System variable `nexial.safari.cleanSession` removed since safari now ALWAYS open clean session. - update to [latest version of chromedriver built for electron app](https://github.com/electron/electron/releases/tag/v2.0.4). - update Edge WebDriver to version: 6.17134 - fixed .commons.sh to properly handle situation where a browser can be found in multiple locations. - update code to initialize firefox and geckodriver; no more deprecated calls. - when checking for browser and webdriver readiness, treat "unexpected end of stream on Connection" NOT as fatal so that Nexial can avoid opening new browser. - added settings to firefox to favor tab over windows - added settings to firefox to allow windows to be closed via JavaScript.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAEC4AB-0A48-0442-80A1-53A22E397E6A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC540C3F-914B-BB46-97DC-3B0B9C193F12}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="31460" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="31460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -8934,9 +8934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11884,9 +11884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DF1F0F-B282-0943-91B8-08553FB5A8B7}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+    <sheetView zoomScale="164" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[Nexial Filter] - new unary filter to simplify boolean filter conditions.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11104"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0843F464-120A-944C-B48A-510FEADC31EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A66240-36ED-CD44-A606-D369E3D4B611}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12520" yWindow="440" windowWidth="38680" windowHeight="15760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12520" yWindow="440" windowWidth="38680" windowHeight="15760" tabRatio="500" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="953">
   <si>
     <t>description</t>
   </si>
@@ -1706,19 +1706,10 @@
     <t>data1 should have skipped this step; it's value is ${data1}</t>
   </si>
   <si>
-    <t>endif</t>
-  </si>
-  <si>
-    <t>data1 should have ended this test without failure; it's value is ${data1}</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>right now data1 is ${data1}</t>
-  </si>
-  <si>
-    <t>should have never got here</t>
   </si>
   <si>
     <t>assertNotContains(text,substring)</t>
@@ -2044,9 +2035,6 @@
   </si>
   <si>
     <t>SkipIf( ${data1}="5" )</t>
-  </si>
-  <si>
-    <t>EndIf( ${data1}="6" )</t>
   </si>
   <si>
     <t>jms</t>
@@ -2999,6 +2987,45 @@
   </si>
   <si>
     <t>colorbit(source,bit,saveTo)</t>
+  </si>
+  <si>
+    <t>unary filter</t>
+  </si>
+  <si>
+    <t>This works!</t>
+  </si>
+  <si>
+    <t>ProceedIf(true)</t>
+  </si>
+  <si>
+    <t>continue?</t>
+  </si>
+  <si>
+    <t>This also works!</t>
+  </si>
+  <si>
+    <t>ProceedIf(${continue?})</t>
+  </si>
+  <si>
+    <t>ProceedIf(!${continue?})</t>
+  </si>
+  <si>
+    <t>This also should not work</t>
+  </si>
+  <si>
+    <t>This should not work</t>
+  </si>
+  <si>
+    <t>This definitely should not work</t>
+  </si>
+  <si>
+    <t>ProceedIf( not ${continue?} )</t>
+  </si>
+  <si>
+    <t>ProceedIf( false )</t>
+  </si>
+  <si>
+    <t>ProceedIf( true &amp; !${continue?} )</t>
   </si>
 </sst>
 </file>
@@ -4327,10 +4354,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C1" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
@@ -4354,7 +4381,7 @@
         <v>145</v>
       </c>
       <c r="K1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="L1" t="s">
         <v>186</v>
@@ -4372,19 +4399,19 @@
         <v>185</v>
       </c>
       <c r="Q1" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="R1" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="S1" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="T1" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="U1" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="V1" t="s">
         <v>32</v>
@@ -4399,7 +4426,7 @@
         <v>132</v>
       </c>
       <c r="Z1" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="AA1" t="s">
         <v>487</v>
@@ -4407,13 +4434,13 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="B2" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="C2" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
@@ -4425,28 +4452,28 @@
         <v>157</v>
       </c>
       <c r="G2" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="H2" t="s">
         <v>146</v>
       </c>
       <c r="I2" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="J2" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="K2" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="L2" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="M2" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="N2" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="O2" t="s">
         <v>530</v>
@@ -4455,19 +4482,19 @@
         <v>401</v>
       </c>
       <c r="Q2" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="R2" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="S2" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="T2" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="U2" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="V2" t="s">
         <v>45</v>
@@ -4482,7 +4509,7 @@
         <v>134</v>
       </c>
       <c r="Z2" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="AA2" t="s">
         <v>488</v>
@@ -4490,19 +4517,19 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="B3" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="C3" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="D3" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="E3" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="F3" t="s">
         <v>180</v>
@@ -4514,19 +4541,19 @@
         <v>147</v>
       </c>
       <c r="I3" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="J3" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="K3" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="L3" t="s">
         <v>187</v>
       </c>
       <c r="N3" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="O3" t="s">
         <v>517</v>
@@ -4535,16 +4562,16 @@
         <v>402</v>
       </c>
       <c r="Q3" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="S3" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="T3" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="U3" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="V3" t="s">
         <v>46</v>
@@ -4556,7 +4583,7 @@
         <v>126</v>
       </c>
       <c r="Y3" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="Z3" t="s">
         <v>133</v>
@@ -4570,7 +4597,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -4579,19 +4606,19 @@
         <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="G4" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="I4" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="J4" t="s">
         <v>515</v>
       </c>
       <c r="K4" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="L4" t="s">
         <v>188</v>
@@ -4606,19 +4633,19 @@
         <v>403</v>
       </c>
       <c r="Q4" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="S4" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="T4" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="U4" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="V4" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="W4" t="s">
         <v>122</v>
@@ -4630,7 +4657,7 @@
         <v>133</v>
       </c>
       <c r="Z4" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="AA4" t="s">
         <v>490</v>
@@ -4641,25 +4668,25 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D5" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="E5" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="F5" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="G5" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I5" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="J5" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="L5" t="s">
         <v>189</v>
@@ -4674,16 +4701,16 @@
         <v>404</v>
       </c>
       <c r="Q5" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="S5" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="T5" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="V5" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="W5" t="s">
         <v>123</v>
@@ -4695,7 +4722,7 @@
         <v>135</v>
       </c>
       <c r="Z5" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="AA5" t="s">
         <v>491</v>
@@ -4706,19 +4733,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="G6" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="I6" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="J6" t="s">
         <v>177</v>
@@ -4733,19 +4760,19 @@
         <v>520</v>
       </c>
       <c r="P6" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="Q6" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="T6" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="V6" t="s">
         <v>47</v>
       </c>
       <c r="W6" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="X6" t="s">
         <v>129</v>
@@ -4754,7 +4781,7 @@
         <v>136</v>
       </c>
       <c r="Z6" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="AA6" t="s">
         <v>492</v>
@@ -4765,22 +4792,22 @@
         <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="D7" t="s">
         <v>457</v>
       </c>
       <c r="F7" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="G7" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="J7" t="s">
         <v>148</v>
       </c>
       <c r="L7" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="N7" t="s">
         <v>24</v>
@@ -4789,19 +4816,19 @@
         <v>521</v>
       </c>
       <c r="P7" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="Q7" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="T7" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="V7" t="s">
         <v>48</v>
       </c>
       <c r="W7" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="X7" t="s">
         <v>130</v>
@@ -4810,7 +4837,7 @@
         <v>137</v>
       </c>
       <c r="Z7" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="AA7" t="s">
         <v>493</v>
@@ -4821,16 +4848,16 @@
         <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="D8" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F8" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="G8" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="J8" t="s">
         <v>170</v>
@@ -4845,10 +4872,10 @@
         <v>522</v>
       </c>
       <c r="Q8" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="T8" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="V8" t="s">
         <v>49</v>
@@ -4863,7 +4890,7 @@
         <v>138</v>
       </c>
       <c r="Z8" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="AA8" t="s">
         <v>494</v>
@@ -4874,16 +4901,16 @@
         <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G9" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="J9" t="s">
         <v>149</v>
@@ -4898,10 +4925,10 @@
         <v>523</v>
       </c>
       <c r="Q9" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="T9" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="V9" t="s">
         <v>210</v>
@@ -4918,31 +4945,31 @@
         <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="F10" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="G10" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="J10" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="L10" t="s">
         <v>193</v>
       </c>
       <c r="N10" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="O10" t="s">
         <v>524</v>
       </c>
       <c r="Q10" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="V10" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="Y10" t="s">
         <v>184</v>
@@ -4953,22 +4980,22 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D11" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="F11" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="G11" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="J11" t="s">
         <v>150</v>
       </c>
       <c r="L11" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="N11" t="s">
         <v>166</v>
@@ -4977,10 +5004,10 @@
         <v>525</v>
       </c>
       <c r="V11" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="Y11" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="AA11" t="s">
         <v>497</v>
@@ -4991,13 +5018,13 @@
         <v>186</v>
       </c>
       <c r="D12" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="F12" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="G12" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="J12" t="s">
         <v>151</v>
@@ -5023,13 +5050,13 @@
         <v>197</v>
       </c>
       <c r="D13" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="F13" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G13" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="J13" t="s">
         <v>171</v>
@@ -5044,7 +5071,7 @@
         <v>531</v>
       </c>
       <c r="V13" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="Y13" t="s">
         <v>140</v>
@@ -5058,10 +5085,10 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="G14" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="J14" t="s">
         <v>172</v>
@@ -5090,10 +5117,10 @@
         <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="J15" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="N15" t="s">
         <v>169</v>
@@ -5113,10 +5140,10 @@
         <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="F16" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="J16" t="s">
         <v>173</v>
@@ -5133,10 +5160,10 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D17" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="F17" t="s">
         <v>181</v>
@@ -5148,21 +5175,21 @@
         <v>53</v>
       </c>
       <c r="Y17" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="D18" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="F18" t="s">
         <v>182</v>
       </c>
       <c r="J18" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="V18" t="s">
         <v>54</v>
@@ -5170,13 +5197,13 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="D19" t="s">
         <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J19" t="s">
         <v>152</v>
@@ -5187,16 +5214,16 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="J20" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="V20" t="s">
         <v>56</v>
@@ -5204,13 +5231,13 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D21" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F21" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="J21" t="s">
         <v>153</v>
@@ -5227,10 +5254,10 @@
         <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="J22" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="V22" t="s">
         <v>58</v>
@@ -5241,10 +5268,10 @@
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="F23" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J23" t="s">
         <v>154</v>
@@ -5261,7 +5288,7 @@
         <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="J24" t="s">
         <v>155</v>
@@ -5275,7 +5302,7 @@
         <v>132</v>
       </c>
       <c r="D25" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="F25" t="s">
         <v>158</v>
@@ -5286,13 +5313,13 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D26" t="s">
         <v>458</v>
       </c>
       <c r="F26" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="V26" t="s">
         <v>62</v>
@@ -5306,18 +5333,18 @@
         <v>459</v>
       </c>
       <c r="F27" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="V27" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="F28" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V28" t="s">
         <v>63</v>
@@ -5328,7 +5355,7 @@
         <v>160</v>
       </c>
       <c r="F29" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="V29" t="s">
         <v>64</v>
@@ -5350,7 +5377,7 @@
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V31" t="s">
         <v>66</v>
@@ -5361,7 +5388,7 @@
         <v>161</v>
       </c>
       <c r="F32" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="V32" t="s">
         <v>67</v>
@@ -5372,7 +5399,7 @@
         <v>162</v>
       </c>
       <c r="F33" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="V33" t="s">
         <v>68</v>
@@ -5383,7 +5410,7 @@
         <v>163</v>
       </c>
       <c r="F34" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="V34" t="s">
         <v>211</v>
@@ -5394,7 +5421,7 @@
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="V35" t="s">
         <v>69</v>
@@ -5405,26 +5432,26 @@
         <v>156</v>
       </c>
       <c r="F36" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="V36" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="37" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="V37" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
     </row>
     <row r="38" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="V38" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="39" spans="4:22" x14ac:dyDescent="0.2">
@@ -5445,7 +5472,7 @@
     </row>
     <row r="41" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F41" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="V41" t="s">
         <v>72</v>
@@ -5453,7 +5480,7 @@
     </row>
     <row r="42" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F42" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="V42" t="s">
         <v>73</v>
@@ -5461,7 +5488,7 @@
     </row>
     <row r="43" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F43" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="V43" t="s">
         <v>74</v>
@@ -5469,7 +5496,7 @@
     </row>
     <row r="44" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F44" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="V44" t="s">
         <v>75</v>
@@ -5477,10 +5504,10 @@
     </row>
     <row r="45" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F45" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="V45" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
     </row>
     <row r="46" spans="4:22" x14ac:dyDescent="0.2">
@@ -5493,7 +5520,7 @@
     </row>
     <row r="47" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="V47" t="s">
         <v>76</v>
@@ -5501,7 +5528,7 @@
     </row>
     <row r="48" spans="4:22" x14ac:dyDescent="0.2">
       <c r="F48" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="V48" t="s">
         <v>77</v>
@@ -5509,7 +5536,7 @@
     </row>
     <row r="49" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F49" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="V49" t="s">
         <v>78</v>
@@ -5517,7 +5544,7 @@
     </row>
     <row r="50" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F50" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="V50" t="s">
         <v>79</v>
@@ -5525,15 +5552,15 @@
     </row>
     <row r="51" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F51" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="V51" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="52" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F52" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="V52" t="s">
         <v>80</v>
@@ -5541,23 +5568,23 @@
     </row>
     <row r="53" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F53" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="V53" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="54" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F54" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="V54" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
     </row>
     <row r="55" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F55" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="V55" t="s">
         <v>81</v>
@@ -5565,7 +5592,7 @@
     </row>
     <row r="56" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F56" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="V56" t="s">
         <v>82</v>
@@ -5573,7 +5600,7 @@
     </row>
     <row r="57" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F57" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="V57" t="s">
         <v>83</v>
@@ -5581,7 +5608,7 @@
     </row>
     <row r="58" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F58" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="V58" t="s">
         <v>84</v>
@@ -5589,7 +5616,7 @@
     </row>
     <row r="59" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F59" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="V59" t="s">
         <v>85</v>
@@ -5597,7 +5624,7 @@
     </row>
     <row r="60" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F60" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="V60" t="s">
         <v>86</v>
@@ -5605,7 +5632,7 @@
     </row>
     <row r="61" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F61" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="V61" t="s">
         <v>87</v>
@@ -5613,15 +5640,15 @@
     </row>
     <row r="62" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F62" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="V62" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="63" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F63" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="V63" t="s">
         <v>399</v>
@@ -5629,23 +5656,23 @@
     </row>
     <row r="64" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F64" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="V64" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
     </row>
     <row r="65" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F65" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="V65" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
     <row r="66" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F66" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="V66" t="s">
         <v>88</v>
@@ -5653,7 +5680,7 @@
     </row>
     <row r="67" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F67" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="V67" t="s">
         <v>89</v>
@@ -5661,7 +5688,7 @@
     </row>
     <row r="68" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F68" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="V68" t="s">
         <v>90</v>
@@ -5669,7 +5696,7 @@
     </row>
     <row r="69" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F69" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="V69" t="s">
         <v>91</v>
@@ -5677,7 +5704,7 @@
     </row>
     <row r="70" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F70" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="V70" t="s">
         <v>198</v>
@@ -5685,7 +5712,7 @@
     </row>
     <row r="71" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F71" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="V71" t="s">
         <v>199</v>
@@ -5693,15 +5720,15 @@
     </row>
     <row r="72" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F72" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="V72" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
     </row>
     <row r="73" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F73" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="V73" t="s">
         <v>92</v>
@@ -5709,7 +5736,7 @@
     </row>
     <row r="74" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F74" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="V74" t="s">
         <v>93</v>
@@ -5717,7 +5744,7 @@
     </row>
     <row r="75" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F75" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="V75" t="s">
         <v>94</v>
@@ -5725,7 +5752,7 @@
     </row>
     <row r="76" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F76" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="V76" t="s">
         <v>95</v>
@@ -5733,7 +5760,7 @@
     </row>
     <row r="77" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F77" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="V77" t="s">
         <v>96</v>
@@ -5741,7 +5768,7 @@
     </row>
     <row r="78" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F78" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="V78" t="s">
         <v>200</v>
@@ -5749,7 +5776,7 @@
     </row>
     <row r="79" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F79" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="V79" t="s">
         <v>201</v>
@@ -5757,15 +5784,15 @@
     </row>
     <row r="80" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F80" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="V80" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="81" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F81" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="V81" t="s">
         <v>202</v>
@@ -5773,7 +5800,7 @@
     </row>
     <row r="82" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F82" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V82" t="s">
         <v>203</v>
@@ -5781,7 +5808,7 @@
     </row>
     <row r="83" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F83" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="V83" t="s">
         <v>400</v>
@@ -5789,7 +5816,7 @@
     </row>
     <row r="84" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F84" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="V84" t="s">
         <v>97</v>
@@ -5797,7 +5824,7 @@
     </row>
     <row r="85" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="V85" t="s">
         <v>204</v>
@@ -5805,23 +5832,23 @@
     </row>
     <row r="86" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V86" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="87" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F87" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="V87" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
     </row>
     <row r="88" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F88" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="V88" t="s">
         <v>205</v>
@@ -5829,7 +5856,7 @@
     </row>
     <row r="89" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="V89" t="s">
         <v>206</v>
@@ -5837,7 +5864,7 @@
     </row>
     <row r="90" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F90" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="V90" t="s">
         <v>207</v>
@@ -5845,7 +5872,7 @@
     </row>
     <row r="91" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F91" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V91" t="s">
         <v>208</v>
@@ -5853,7 +5880,7 @@
     </row>
     <row r="92" spans="6:22" x14ac:dyDescent="0.2">
       <c r="F92" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="V92" t="s">
         <v>456</v>
@@ -5871,7 +5898,7 @@
     </row>
     <row r="95" spans="6:22" x14ac:dyDescent="0.2">
       <c r="V95" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="96" spans="6:22" x14ac:dyDescent="0.2">
@@ -5941,7 +5968,7 @@
     </row>
     <row r="109" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V109" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
     </row>
     <row r="110" spans="22:22" x14ac:dyDescent="0.2">
@@ -6034,10 +6061,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -6136,7 +6163,7 @@
     </row>
     <row r="5" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
@@ -6146,14 +6173,14 @@
         <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="24" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="14"/>
@@ -6168,16 +6195,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>552</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -6191,7 +6218,7 @@
     <row r="7" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>13</v>
@@ -6200,7 +6227,7 @@
         <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -6216,7 +6243,7 @@
     <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>13</v>
@@ -6225,7 +6252,7 @@
         <v>43</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -6240,25 +6267,25 @@
     </row>
     <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>549</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>552</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -6272,16 +6299,16 @@
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" s="57" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -6301,7 +6328,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
@@ -6320,13 +6347,13 @@
         <v>13</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>395</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -6338,7 +6365,7 @@
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" s="8" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>31</v>
@@ -6347,7 +6374,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>395</v>
@@ -6362,7 +6389,7 @@
     <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" s="8" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>31</v>
@@ -6371,10 +6398,10 @@
         <v>26</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -6386,7 +6413,7 @@
     <row r="15" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" s="8" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>13</v>
@@ -6395,7 +6422,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -6407,10 +6434,10 @@
     </row>
     <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>13</v>
@@ -6419,7 +6446,7 @@
         <v>43</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -6432,27 +6459,27 @@
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17" s="8" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17" s="25" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="K17"/>
       <c r="L17"/>
@@ -6460,7 +6487,7 @@
     <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18" s="8" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>13</v>
@@ -6469,7 +6496,7 @@
         <v>43</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -6482,13 +6509,13 @@
     <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19" s="8" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -6511,7 +6538,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -6524,7 +6551,7 @@
     <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21" s="8" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>13</v>
@@ -6533,7 +6560,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -6546,19 +6573,19 @@
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22" s="8" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
@@ -6570,7 +6597,7 @@
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="8" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>13</v>
@@ -6579,7 +6606,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
@@ -6591,19 +6618,19 @@
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
@@ -6616,7 +6643,7 @@
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="8" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>13</v>
@@ -6625,7 +6652,7 @@
         <v>43</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="F25"/>
       <c r="G25"/>
@@ -6645,7 +6672,7 @@
         <v>40</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>282</v>
@@ -6660,19 +6687,19 @@
     <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27" s="8" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>395</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
@@ -6684,7 +6711,7 @@
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="8" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>31</v>
@@ -6693,7 +6720,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>395</v>
@@ -6708,7 +6735,7 @@
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29" s="8" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>13</v>
@@ -6717,7 +6744,7 @@
         <v>43</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="F29"/>
       <c r="G29"/>
@@ -6730,7 +6757,7 @@
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="8" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>31</v>
@@ -6739,10 +6766,10 @@
         <v>26</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -6754,7 +6781,7 @@
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31" s="8" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>13</v>
@@ -6763,7 +6790,7 @@
         <v>43</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="F31"/>
       <c r="G31"/>
@@ -6847,10 +6874,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -6949,7 +6976,7 @@
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
@@ -6959,7 +6986,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>282</v>
@@ -6984,7 +7011,7 @@
         <v>43</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -7000,19 +7027,19 @@
     <row r="7" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>232</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -7027,19 +7054,19 @@
     <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -7054,7 +7081,7 @@
     <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>13</v>
@@ -7063,7 +7090,7 @@
         <v>156</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -7079,7 +7106,7 @@
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>13</v>
@@ -7088,7 +7115,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -7104,7 +7131,7 @@
     <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="27" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>31</v>
@@ -7113,10 +7140,10 @@
         <v>26</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -7131,7 +7158,7 @@
     <row r="12" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>145</v>
@@ -7140,10 +7167,10 @@
         <v>153</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>238</v>
@@ -7159,7 +7186,7 @@
     </row>
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="12" t="s">
@@ -7169,7 +7196,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -7185,7 +7212,7 @@
     <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>145</v>
@@ -7194,10 +7221,10 @@
         <v>171</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -7219,7 +7246,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -7305,10 +7332,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -7324,7 +7351,7 @@
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B2" s="64"/>
       <c r="C2" s="64"/>
@@ -7407,7 +7434,7 @@
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="36" t="s">
@@ -7417,10 +7444,10 @@
         <v>40</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
@@ -7442,10 +7469,10 @@
         <v>40</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
@@ -7467,7 +7494,7 @@
         <v>43</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
@@ -7490,7 +7517,7 @@
         <v>43</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
@@ -7513,7 +7540,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -7529,7 +7556,7 @@
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="53"/>
       <c r="B10" s="39" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>13</v>
@@ -7538,7 +7565,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>230</v>
@@ -7563,10 +7590,10 @@
         <v>40</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
@@ -7581,7 +7608,7 @@
     <row r="12" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="53"/>
       <c r="B12" s="33" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>13</v>
@@ -7590,7 +7617,7 @@
         <v>43</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -7606,7 +7633,7 @@
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="53"/>
       <c r="B13" s="33" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>13</v>
@@ -7615,7 +7642,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -7630,7 +7657,7 @@
     </row>
     <row r="14" spans="1:15" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="53" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="36" t="s">
@@ -7640,10 +7667,10 @@
         <v>40</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
@@ -7665,7 +7692,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
@@ -7680,7 +7707,7 @@
     </row>
     <row r="16" spans="1:15" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="36" t="s">
@@ -7690,10 +7717,10 @@
         <v>40</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
@@ -7715,7 +7742,7 @@
         <v>43</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
@@ -7730,7 +7757,7 @@
     </row>
     <row r="18" spans="1:15" ht="273" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="53" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="36" t="s">
@@ -7740,10 +7767,10 @@
         <v>40</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
@@ -7758,7 +7785,7 @@
     <row r="19" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="53"/>
       <c r="B19" s="33" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C19" s="36" t="s">
         <v>13</v>
@@ -7767,7 +7794,7 @@
         <v>43</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="F19" s="40"/>
       <c r="G19" s="37"/>
@@ -7790,7 +7817,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="F20" s="40"/>
       <c r="G20" s="37"/>
@@ -7813,7 +7840,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
@@ -7829,7 +7856,7 @@
     <row r="22" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="53"/>
       <c r="B22" s="33" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="C22" s="36" t="s">
         <v>186</v>
@@ -7838,13 +7865,13 @@
         <v>196</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
@@ -7865,7 +7892,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
@@ -7880,7 +7907,7 @@
     </row>
     <row r="24" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="53" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="36" t="s">
@@ -7890,10 +7917,10 @@
         <v>40</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
@@ -7915,7 +7942,7 @@
         <v>43</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="37"/>
@@ -7938,7 +7965,7 @@
         <v>43</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
@@ -7961,7 +7988,7 @@
         <v>43</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
@@ -7976,7 +8003,7 @@
     </row>
     <row r="28" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="53" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="36" t="s">
@@ -7986,7 +8013,7 @@
         <v>43</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
@@ -8002,7 +8029,7 @@
     <row r="29" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="53"/>
       <c r="B29" s="33" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C29" s="36" t="s">
         <v>145</v>
@@ -8011,10 +8038,10 @@
         <v>153</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>244</v>
@@ -8038,10 +8065,10 @@
         <v>153</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>238</v>
@@ -8065,10 +8092,10 @@
         <v>171</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="G31" s="37"/>
       <c r="H31" s="37"/>
@@ -8090,10 +8117,10 @@
         <v>457</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="G32" s="37" t="s">
         <v>420</v>
@@ -8117,7 +8144,7 @@
         <v>43</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
@@ -8132,10 +8159,10 @@
     </row>
     <row r="34" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="53" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>13</v>
@@ -8144,10 +8171,10 @@
         <v>40</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="G34" s="37"/>
       <c r="H34" s="37"/>
@@ -8169,10 +8196,10 @@
         <v>153</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>238</v>
@@ -8196,10 +8223,10 @@
         <v>153</v>
       </c>
       <c r="E36" s="37" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="G36" s="37" t="s">
         <v>238</v>
@@ -8223,10 +8250,10 @@
         <v>153</v>
       </c>
       <c r="E37" s="37" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="G37" s="37" t="s">
         <v>238</v>
@@ -8250,10 +8277,10 @@
         <v>153</v>
       </c>
       <c r="E38" s="37" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>238</v>
@@ -8277,7 +8304,7 @@
         <v>43</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="F39" s="37"/>
       <c r="G39" s="37"/>
@@ -8300,7 +8327,7 @@
         <v>43</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="37"/>
@@ -8316,7 +8343,7 @@
     <row r="41" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="53"/>
       <c r="B41" s="33" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C41" s="36" t="s">
         <v>13</v>
@@ -8325,10 +8352,10 @@
         <v>40</v>
       </c>
       <c r="E41" s="37" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="G41" s="37"/>
       <c r="H41" s="37"/>
@@ -8350,7 +8377,7 @@
         <v>43</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="F42" s="37"/>
       <c r="G42" s="37"/>
@@ -8454,10 +8481,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -8554,20 +8581,20 @@
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -8586,13 +8613,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -8611,13 +8638,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -8636,13 +8663,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -8661,13 +8688,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -8713,11 +8740,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8752,10 +8779,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -8900,7 +8927,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="24" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="14"/>
@@ -8923,7 +8950,7 @@
         <v>540</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -8945,7 +8972,7 @@
         <v>43</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -8960,7 +8987,7 @@
     </row>
     <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>539</v>
@@ -8972,10 +8999,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>232</v>
+        <v>364</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -8990,19 +9017,19 @@
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>483</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -9017,7 +9044,7 @@
     <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>13</v>
@@ -9026,14 +9053,14 @@
         <v>43</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="24" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="14"/>
@@ -9051,7 +9078,7 @@
         <v>43</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -9065,16 +9092,26 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>940</v>
+      </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="C13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>941</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="24"/>
+      <c r="J13" s="24" t="s">
+        <v>942</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="14"/>
       <c r="M13" s="11"/>
@@ -9084,10 +9121,18 @@
     <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>943</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>238</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -9099,27 +9144,23 @@
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>543</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>539</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>544</v>
+        <v>944</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="24" t="s">
-        <v>656</v>
+        <v>945</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="14"/>
@@ -9134,21 +9175,68 @@
         <v>13</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>547</v>
+        <v>948</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="24"/>
+      <c r="J16" s="24" t="s">
+        <v>946</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="L16" s="14"/>
       <c r="M16" s="11"/>
       <c r="N16" s="14"/>
       <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>947</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>949</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>951</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
@@ -9187,7 +9275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
@@ -9223,10 +9311,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -9337,7 +9425,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F5" s="56"/>
       <c r="G5" s="56"/>
@@ -9419,7 +9507,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="24" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="14"/>
@@ -9484,7 +9572,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>221</v>
@@ -9509,7 +9597,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>219</v>
@@ -9561,7 +9649,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>221</v>
@@ -9638,7 +9726,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>221</v>
@@ -9765,7 +9853,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>217</v>
@@ -9978,7 +10066,7 @@
         <v>40</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>246</v>
@@ -10137,7 +10225,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>259</v>
@@ -10191,7 +10279,7 @@
         <v>13</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>264</v>
@@ -10247,7 +10335,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>269</v>
@@ -10299,7 +10387,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>273</v>
@@ -10355,7 +10443,7 @@
         <v>13</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>453</v>
@@ -10439,7 +10527,7 @@
         <v>40</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>282</v>
@@ -10448,7 +10536,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="14"/>
@@ -10468,7 +10556,7 @@
         <v>40</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>284</v>
@@ -10477,7 +10565,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="14"/>
@@ -10497,7 +10585,7 @@
         <v>40</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>286</v>
@@ -10506,7 +10594,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="14"/>
@@ -10526,7 +10614,7 @@
         <v>40</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>288</v>
@@ -10535,7 +10623,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="14"/>
@@ -10560,7 +10648,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="14"/>
@@ -10580,7 +10668,7 @@
         <v>40</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>282</v>
@@ -10609,7 +10697,7 @@
         <v>43</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -10634,7 +10722,7 @@
         <v>20</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>294</v>
@@ -10661,7 +10749,7 @@
         <v>43</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -10686,7 +10774,7 @@
         <v>43</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -10810,7 +10898,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
       <c r="J61" s="24" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="K61" s="2"/>
       <c r="L61" s="14"/>
@@ -10852,7 +10940,7 @@
         <v>13</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>306</v>
@@ -10877,7 +10965,7 @@
         <v>13</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>308</v>
@@ -10902,7 +10990,7 @@
         <v>13</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>310</v>
@@ -10927,7 +11015,7 @@
         <v>13</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>312</v>
@@ -10952,7 +11040,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>314</v>
@@ -10977,7 +11065,7 @@
         <v>13</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>316</v>
@@ -11002,7 +11090,7 @@
         <v>13</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>318</v>
@@ -11027,7 +11115,7 @@
         <v>13</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>320</v>
@@ -11052,7 +11140,7 @@
         <v>13</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>322</v>
@@ -11077,7 +11165,7 @@
         <v>13</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>324</v>
@@ -11102,7 +11190,7 @@
         <v>13</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>326</v>
@@ -11127,7 +11215,7 @@
         <v>13</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>328</v>
@@ -11152,7 +11240,7 @@
         <v>13</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>330</v>
@@ -11392,13 +11480,13 @@
     <row r="85" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>345</v>
@@ -11410,7 +11498,7 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
       <c r="J85" s="24" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="K85" s="2"/>
       <c r="L85" s="14"/>
@@ -11421,13 +11509,13 @@
     <row r="86" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>477</v>
@@ -11439,7 +11527,7 @@
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
       <c r="J86" s="24" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="K86" s="2"/>
       <c r="L86" s="14"/>
@@ -11599,10 +11687,10 @@
         <v>460</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
@@ -11624,7 +11712,7 @@
         <v>13</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>483</v>
@@ -11636,7 +11724,7 @@
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
       <c r="J93" s="24" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="K93" s="2"/>
       <c r="L93" s="14"/>
@@ -11651,7 +11739,7 @@
         <v>31</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>484</v>
@@ -11663,7 +11751,7 @@
       <c r="H94" s="6"/>
       <c r="I94" s="6"/>
       <c r="J94" s="24" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="K94" s="2"/>
       <c r="L94" s="14"/>
@@ -11680,7 +11768,7 @@
         <v>31</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>485</v>
@@ -11803,10 +11891,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -11915,7 +12003,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>238</v>
@@ -12019,7 +12107,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>537</v>
@@ -12043,7 +12131,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>355</v>
@@ -12177,10 +12265,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -12279,7 +12367,7 @@
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
@@ -12289,7 +12377,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -12312,7 +12400,7 @@
         <v>40</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>246</v>
@@ -12337,14 +12425,14 @@
         <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="24" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="14"/>
@@ -12917,10 +13005,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -13029,7 +13117,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>230</v>
@@ -13076,7 +13164,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>359</v>
@@ -13101,7 +13189,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>361</v>
@@ -13126,7 +13214,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>363</v>
@@ -13151,7 +13239,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>365</v>
@@ -13176,7 +13264,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>367</v>
@@ -13201,7 +13289,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>369</v>
@@ -13226,7 +13314,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>371</v>
@@ -13251,7 +13339,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>373</v>
@@ -13276,7 +13364,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>375</v>
@@ -13326,7 +13414,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>379</v>
@@ -13351,7 +13439,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>381</v>
@@ -13376,7 +13464,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>383</v>
@@ -13401,7 +13489,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>385</v>
@@ -13426,7 +13514,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>387</v>
@@ -13451,7 +13539,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>389</v>
@@ -13476,7 +13564,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>391</v>
@@ -13501,7 +13589,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>393</v>
@@ -13526,7 +13614,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>394</v>
@@ -13616,10 +13704,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -13728,7 +13816,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>230</v>
@@ -13775,7 +13863,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>359</v>
@@ -13800,7 +13888,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>361</v>
@@ -13825,7 +13913,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>363</v>
@@ -13850,7 +13938,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>365</v>
@@ -13875,7 +13963,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>367</v>
@@ -13900,7 +13988,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>369</v>
@@ -13925,7 +14013,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>371</v>
@@ -13950,7 +14038,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>373</v>
@@ -13975,7 +14063,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>375</v>
@@ -14025,7 +14113,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>379</v>
@@ -14050,7 +14138,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>381</v>
@@ -14075,7 +14163,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>383</v>
@@ -14100,7 +14188,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>385</v>
@@ -14125,7 +14213,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>387</v>
@@ -14150,7 +14238,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>389</v>
@@ -14177,7 +14265,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>462</v>
@@ -14202,7 +14290,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>463</v>
@@ -14227,7 +14315,7 @@
         <v>31</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>465</v>
@@ -14252,7 +14340,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>466</v>
@@ -14277,7 +14365,7 @@
         <v>31</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>468</v>
@@ -14302,7 +14390,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>469</v>
@@ -14327,7 +14415,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>470</v>
@@ -14352,7 +14440,7 @@
         <v>31</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>471</v>
@@ -14377,7 +14465,7 @@
         <v>31</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>473</v>
@@ -14402,7 +14490,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>474</v>
@@ -14422,7 +14510,7 @@
     </row>
     <row r="33" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="12" t="s">
@@ -14432,7 +14520,7 @@
         <v>43</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -14567,10 +14655,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -15750,10 +15838,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -15914,7 +16002,7 @@
         <v>40</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>230</v>
@@ -15965,7 +16053,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>418</v>
@@ -15990,7 +16078,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>434</v>
@@ -16171,7 +16259,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>418</v>
@@ -16391,10 +16479,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -16546,7 +16634,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>535</v>
@@ -16566,7 +16654,7 @@
     </row>
     <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="12" t="s">
@@ -16576,7 +16664,7 @@
         <v>43</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -16596,13 +16684,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>

</xml_diff>

<commit_message>
- support skipping of command via "strikethrough": Use `Ctrl-5` on a "command" column to skip over the corresponding   test step. This effectively add a `SkipIf(true)` flow control to the corresponding "flow controls" column.   Use `Ctrl-5` again to enable the corresponding test step.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11202"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A66240-36ED-CD44-A606-D369E3D4B611}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2B472A-C0E0-4343-A872-9344D7BAFD22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12520" yWindow="440" windowWidth="38680" windowHeight="15760" tabRatio="500" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="440" windowWidth="38680" windowHeight="15760" tabRatio="500" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="expression-test" sheetId="15" r:id="rId12"/>
     <sheet name="multi-scenario2" sheetId="17" r:id="rId13"/>
     <sheet name="flow_controls" sheetId="12" r:id="rId14"/>
+    <sheet name="temp_disable" sheetId="19" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
@@ -67,6 +68,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -75,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="962">
   <si>
     <t>description</t>
   </si>
@@ -3027,12 +3033,39 @@
   <si>
     <t>ProceedIf( true &amp; !${continue?} )</t>
   </si>
+  <si>
+    <t>showcase/testing out how to disable one or more steps</t>
+  </si>
+  <si>
+    <t>Act 1</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>-31</t>
+  </si>
+  <si>
+    <t>${result}</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>-12</t>
+  </si>
+  <si>
+    <t>Act 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3141,6 +3174,25 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Consolas"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3370,7 +3422,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3573,6 +3625,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3624,6 +3682,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -3659,7 +3726,37 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4054,6 +4151,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFE6E6E6"/>
       <color rgb="FFF8F7F9"/>
       <color rgb="FFF5F4F6"/>
       <color rgb="FFE6EDF1"/>
@@ -6048,12 +6146,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -6071,20 +6169,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -6094,10 +6192,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -6809,13 +6907,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="16" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="15" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6861,12 +6959,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -6884,20 +6982,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -6907,10 +7005,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -7268,13 +7366,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="12" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7319,12 +7417,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="51" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -7342,20 +7440,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>831</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -7365,10 +7463,10 @@
       </c>
       <c r="J2" s="30"/>
       <c r="K2" s="31"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="72"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:15" s="51" customFormat="1" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
@@ -8417,13 +8515,13 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8468,12 +8566,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -8491,18 +8589,18 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -8512,10 +8610,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -8715,13 +8813,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="7" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8742,9 +8840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8766,12 +8864,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -8789,20 +8887,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>405</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -8812,10 +8910,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -9238,6 +9336,297 @@
         <v>951</v>
       </c>
     </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N1 N3:N1048576">
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+      <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+      <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+      <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1048576" xr:uid="{00000000-0002-0000-0D00-000001000000}">
+      <formula1>target</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+      <formula1>INDIRECT(C5)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D87D36E-04A6-D640-B45B-3F4AC7187531}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.83203125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="9" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.6640625" style="25" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="1.6640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" style="15" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.5" style="16" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.83203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="49.83203125" style="10" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>803</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
+    </row>
+    <row r="2" spans="1:15" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>953</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
+    </row>
+    <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>435</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>905</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>958</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>958</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -9258,11 +9647,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1048576" xr:uid="{00000000-0002-0000-0D00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{1F6843CC-2858-5C42-AC22-AD86AE7F9E69}">
+      <formula1>INDIRECT(C5)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1048576" xr:uid="{884DE651-E754-374E-8C50-AD3752225945}">
       <formula1>target</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{00000000-0002-0000-0D00-000000000000}">
-      <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9298,12 +9687,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -9321,20 +9710,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -9344,10 +9733,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -11829,13 +12218,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="38" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="41" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="37" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="40" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="39" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11878,12 +12267,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -11901,20 +12290,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -11924,10 +12313,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -12202,13 +12591,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="35" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="38" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="37" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="36" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12252,12 +12641,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -12275,20 +12664,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -12298,10 +12687,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -12942,13 +13331,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="32" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="35" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="34" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="33" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12992,12 +13381,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -13015,20 +13404,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -13038,10 +13427,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -13641,13 +14030,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="32" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="31" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="30" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13691,12 +14080,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -13714,20 +14103,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -13737,10 +14126,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -14593,13 +14982,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="28" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="27" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14642,12 +15031,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -14665,20 +15054,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -14688,10 +15077,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -15776,13 +16165,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15825,12 +16214,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -15848,20 +16237,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>405</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -15871,10 +16260,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -16415,13 +16804,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="21" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16466,12 +16855,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
@@ -16489,20 +16878,20 @@
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
     </row>
     <row r="2" spans="1:15" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -16512,10 +16901,10 @@
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="70"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -27960,13 +28349,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="19" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="18" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[function] - [`$(date|setDOW|date|day)`](../functions/$(date).md#datesetdowdateday): added boundary checks to ensure meaningful   `day` value. Only 0 through 7 is allowed for the `day` parameter.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FC1876-8DD0-CE4E-92C3-EAA1E7B1B002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F42286-D677-C646-8F1D-DF56751E10BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" tabRatio="500" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="1081">
   <si>
     <t>description</t>
   </si>
@@ -3509,6 +3509,33 @@
   </si>
   <si>
     <t>screenshot(file,locator)</t>
+  </si>
+  <si>
+    <t>Messing with Nexial Mail</t>
+  </si>
+  <si>
+    <t>nexial.mailHeader</t>
+  </si>
+  <si>
+    <t>Check out this &lt;a href="$(syspath|data|fullpath)/dummy.data.csv"&gt;dummy!&lt;/a&gt;&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Make sure email gets sent</t>
+  </si>
+  <si>
+    <t>nexial.enableEmail</t>
+  </si>
+  <si>
+    <t>nexial.mailTo</t>
+  </si>
+  <si>
+    <t>mliu@ep.com</t>
+  </si>
+  <si>
+    <t>Let's see that email now... Give it 5 sec</t>
+  </si>
+  <si>
+    <t>...and how cool is this pix!&lt;br/&gt;&lt;img src="file://$(syspath|data|fullpath)/image-convert-sample.gif"/&gt;&lt;br/&gt;</t>
   </si>
 </sst>
 </file>
@@ -6899,7 +6926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
@@ -21263,14 +21290,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="63" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.1640625" style="63" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.83203125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.5" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="42.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
@@ -22018,17 +22045,85 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="63" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="63" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">

</xml_diff>

<commit_message>
[expression] - [TEXT &raquo; `extract(beginRegex,endRegex,inclusive)`]: **NEW** operation to extract all instances of text between two regex-based patterns as a LIST expression.
[ws]
- [`nexial.ws.logDetail`]: set `true` to log the detail for each web service call.
- [`nexial.ws.logSummary`]: set `true` to log the summary of each web service call.
- code fix to parse empty cookie in response header.
- added `.ttfb` property to the response of web service call (e.g. ``${response}.ttfb`).
- added `.requestTime` property to the Response of web service call (e.g. `${response}.requestTime`).
- ensure the specified response data variable is cleared out prior to web service call, thus preventing previously derived response to be used.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62653F02-13E8-4F44-880A-BDE7E545EE3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D825834-8A6B-9240-9A6B-978123D59DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" tabRatio="500" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="23680" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1095">
   <si>
     <t>description</t>
   </si>
@@ -2474,9 +2474,6 @@
 $(random|alphanumeric|10000)
 $(random|alphanumeric|10000)
 $(random|alphanumeric|3000)</t>
-  </si>
-  <si>
-    <t>$(sysdate|now|MM/dd/yyyy HH:mm:ss.S)${tab}${counter}</t>
   </si>
   <si>
     <t>I love [TEXT(${fruit}) =&gt; append(\,) append(${more fruits}) pack list(\,)] - and they are [TEXT(good for you) =&gt; upper]!</t>
@@ -3539,6 +3536,48 @@
   </si>
   <si>
     <t>saveMatches(var,path,fileFilter,textFilter)</t>
+  </si>
+  <si>
+    <t>Repeat Loop 2</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>current_val</t>
+  </si>
+  <si>
+    <t>${index}</t>
+  </si>
+  <si>
+    <t>${current_val}</t>
+  </si>
+  <si>
+    <t>you feel lucky, jack?!</t>
+  </si>
+  <si>
+    <t>try again</t>
+  </si>
+  <si>
+    <t>magic number</t>
+  </si>
+  <si>
+    <t>$(random|numeric|1|10)</t>
+  </si>
+  <si>
+    <t>$(random|numeric|${index}|10)</t>
+  </si>
+  <si>
+    <t>$(sysdate|now|MM/dd/yyyy HH:mm:ss.S)${tab}${counter}(eol)</t>
+  </si>
+  <si>
+    <t>winning_count</t>
+  </si>
+  <si>
+    <t>ProceedIf( ${nexial.lastOutcome} )</t>
+  </si>
+  <si>
+    <t>You've guessed right ${winning_count} time(s)!</t>
   </si>
 </sst>
 </file>
@@ -4975,13 +5014,13 @@
         <v>747</v>
       </c>
       <c r="C1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -5011,10 +5050,10 @@
         <v>183</v>
       </c>
       <c r="O1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="P1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="Q1" t="s">
         <v>194</v>
@@ -5029,19 +5068,19 @@
         <v>182</v>
       </c>
       <c r="U1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="V1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="W1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="X1" t="s">
         <v>733</v>
       </c>
       <c r="Y1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="Z1" t="s">
         <v>32</v>
@@ -5056,7 +5095,7 @@
         <v>131</v>
       </c>
       <c r="AD1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="AE1" t="s">
         <v>484</v>
@@ -5070,13 +5109,13 @@
         <v>748</v>
       </c>
       <c r="C2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E2" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
@@ -5088,13 +5127,13 @@
         <v>155</v>
       </c>
       <c r="I2" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="J2" t="s">
         <v>145</v>
       </c>
       <c r="K2" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="L2" t="s">
         <v>610</v>
@@ -5103,19 +5142,19 @@
         <v>762</v>
       </c>
       <c r="N2" t="s">
+        <v>894</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="P2" t="s">
+        <v>984</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>825</v>
+      </c>
+      <c r="R2" t="s">
         <v>895</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1026</v>
-      </c>
-      <c r="P2" t="s">
-        <v>985</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>826</v>
-      </c>
-      <c r="R2" t="s">
-        <v>896</v>
       </c>
       <c r="S2" t="s">
         <v>527</v>
@@ -5124,19 +5163,19 @@
         <v>398</v>
       </c>
       <c r="U2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="V2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="W2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X2" t="s">
         <v>759</v>
       </c>
       <c r="Y2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="Z2" t="s">
         <v>45</v>
@@ -5151,27 +5190,27 @@
         <v>133</v>
       </c>
       <c r="AD2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="AE2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B3" t="s">
         <v>749</v>
       </c>
       <c r="C3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G3" t="s">
         <v>741</v>
@@ -5183,7 +5222,7 @@
         <v>176</v>
       </c>
       <c r="J3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="K3" t="s">
         <v>704</v>
@@ -5198,13 +5237,13 @@
         <v>184</v>
       </c>
       <c r="O3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="P3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="R3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="S3" t="s">
         <v>514</v>
@@ -5213,16 +5252,16 @@
         <v>399</v>
       </c>
       <c r="U3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="X3" t="s">
         <v>760</v>
       </c>
       <c r="Y3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="Z3" t="s">
         <v>46</v>
@@ -5245,13 +5284,13 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B4" t="s">
         <v>750</v>
       </c>
       <c r="D4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -5263,10 +5302,10 @@
         <v>766</v>
       </c>
       <c r="I4" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="J4" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="K4" t="s">
         <v>705</v>
@@ -5281,10 +5320,10 @@
         <v>185</v>
       </c>
       <c r="O4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="P4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="R4" t="s">
         <v>19</v>
@@ -5296,16 +5335,16 @@
         <v>400</v>
       </c>
       <c r="U4" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="W4" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="X4" t="s">
         <v>734</v>
       </c>
       <c r="Y4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="Z4" t="s">
         <v>712</v>
@@ -5320,7 +5359,7 @@
         <v>132</v>
       </c>
       <c r="AD4" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="AE4" t="s">
         <v>486</v>
@@ -5328,40 +5367,40 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B5" t="s">
         <v>751</v>
       </c>
       <c r="D5" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F5" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="I5" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="J5" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="K5" t="s">
         <v>706</v>
       </c>
       <c r="L5" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="N5" t="s">
         <v>186</v>
       </c>
       <c r="O5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="R5" t="s">
         <v>21</v>
@@ -5373,16 +5412,16 @@
         <v>401</v>
       </c>
       <c r="U5" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="W5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="X5" t="s">
         <v>735</v>
       </c>
       <c r="Z5" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="AA5" t="s">
         <v>122</v>
@@ -5394,7 +5433,7 @@
         <v>134</v>
       </c>
       <c r="AD5" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="AE5" t="s">
         <v>487</v>
@@ -5408,19 +5447,19 @@
         <v>752</v>
       </c>
       <c r="D6" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="H6" t="s">
         <v>655</v>
       </c>
       <c r="I6" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="K6" t="s">
         <v>703</v>
@@ -5432,7 +5471,7 @@
         <v>187</v>
       </c>
       <c r="O6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R6" t="s">
         <v>22</v>
@@ -5444,7 +5483,7 @@
         <v>770</v>
       </c>
       <c r="U6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="X6" t="s">
         <v>737</v>
@@ -5453,7 +5492,7 @@
         <v>47</v>
       </c>
       <c r="AA6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="AB6" t="s">
         <v>128</v>
@@ -5462,7 +5501,7 @@
         <v>135</v>
       </c>
       <c r="AD6" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AE6" t="s">
         <v>488</v>
@@ -5482,10 +5521,10 @@
         <v>767</v>
       </c>
       <c r="I7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="K7" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="L7" t="s">
         <v>146</v>
@@ -5494,7 +5533,7 @@
         <v>610</v>
       </c>
       <c r="O7" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="R7" t="s">
         <v>24</v>
@@ -5503,10 +5542,10 @@
         <v>518</v>
       </c>
       <c r="T7" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="U7" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="X7" t="s">
         <v>736</v>
@@ -5515,7 +5554,7 @@
         <v>48</v>
       </c>
       <c r="AA7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="AB7" t="s">
         <v>129</v>
@@ -5524,10 +5563,10 @@
         <v>136</v>
       </c>
       <c r="AD7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="AE7" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
@@ -5547,13 +5586,13 @@
         <v>641</v>
       </c>
       <c r="L8" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="N8" t="s">
         <v>188</v>
       </c>
       <c r="O8" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="R8" t="s">
         <v>162</v>
@@ -5562,7 +5601,7 @@
         <v>519</v>
       </c>
       <c r="U8" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="X8" t="s">
         <v>738</v>
@@ -5580,10 +5619,10 @@
         <v>137</v>
       </c>
       <c r="AD8" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AE8" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -5609,7 +5648,7 @@
         <v>189</v>
       </c>
       <c r="O9" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="R9" t="s">
         <v>163</v>
@@ -5618,7 +5657,7 @@
         <v>520</v>
       </c>
       <c r="U9" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="X9" t="s">
         <v>739</v>
@@ -5630,7 +5669,7 @@
         <v>180</v>
       </c>
       <c r="AE9" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
@@ -5644,7 +5683,7 @@
         <v>601</v>
       </c>
       <c r="I10" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L10" t="s">
         <v>147</v>
@@ -5653,16 +5692,16 @@
         <v>190</v>
       </c>
       <c r="O10" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="R10" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="S10" t="s">
         <v>521</v>
       </c>
       <c r="U10" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="Z10" t="s">
         <v>551</v>
@@ -5679,7 +5718,7 @@
         <v>369</v>
       </c>
       <c r="F11" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="H11" t="s">
         <v>707</v>
@@ -5688,13 +5727,13 @@
         <v>635</v>
       </c>
       <c r="L11" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="N11" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="O11" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="R11" t="s">
         <v>164</v>
@@ -5729,10 +5768,10 @@
         <v>769</v>
       </c>
       <c r="N12" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="O12" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="R12" t="s">
         <v>26</v>
@@ -5767,7 +5806,7 @@
         <v>148</v>
       </c>
       <c r="N13" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="R13" t="s">
         <v>165</v>
@@ -5782,7 +5821,7 @@
         <v>139</v>
       </c>
       <c r="AE13" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
@@ -5802,7 +5841,7 @@
         <v>149</v>
       </c>
       <c r="N14" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="R14" t="s">
         <v>166</v>
@@ -5817,12 +5856,12 @@
         <v>140</v>
       </c>
       <c r="AE14" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F15" t="s">
         <v>36</v>
@@ -5831,13 +5870,13 @@
         <v>558</v>
       </c>
       <c r="L15" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="N15" t="s">
         <v>191</v>
       </c>
       <c r="R15" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="S15" t="s">
         <v>525</v>
@@ -5849,12 +5888,12 @@
         <v>141</v>
       </c>
       <c r="AE15" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F16" t="s">
         <v>763</v>
@@ -5866,10 +5905,10 @@
         <v>168</v>
       </c>
       <c r="N16" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="R16" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="S16" t="s">
         <v>526</v>
@@ -5881,7 +5920,7 @@
         <v>142</v>
       </c>
       <c r="AE16" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
@@ -5901,13 +5940,13 @@
         <v>192</v>
       </c>
       <c r="Z17" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="AC17" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="AE17" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
@@ -5915,13 +5954,13 @@
         <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H18" t="s">
         <v>178</v>
       </c>
       <c r="L18" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="N18" t="s">
         <v>193</v>
@@ -5930,7 +5969,7 @@
         <v>53</v>
       </c>
       <c r="AE18" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -5938,7 +5977,7 @@
         <v>513</v>
       </c>
       <c r="F19" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="H19" t="s">
         <v>179</v>
@@ -5950,7 +5989,7 @@
         <v>54</v>
       </c>
       <c r="AE19" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -5970,12 +6009,12 @@
         <v>55</v>
       </c>
       <c r="AE20" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F21" t="s">
         <v>38</v>
@@ -5984,18 +6023,18 @@
         <v>591</v>
       </c>
       <c r="L21" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="Z21" t="s">
         <v>56</v>
       </c>
       <c r="AE21" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F22" t="s">
         <v>542</v>
@@ -6004,10 +6043,10 @@
         <v>592</v>
       </c>
       <c r="L22" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="Z22" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="AE22" t="s">
         <v>492</v>
@@ -6015,10 +6054,10 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F23" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H23" t="s">
         <v>593</v>
@@ -6030,7 +6069,7 @@
         <v>57</v>
       </c>
       <c r="AE23" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
@@ -6047,15 +6086,15 @@
         <v>771</v>
       </c>
       <c r="Z24" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="AE24" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F25" t="s">
         <v>624</v>
@@ -6064,13 +6103,13 @@
         <v>573</v>
       </c>
       <c r="L25" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="Z25" t="s">
         <v>58</v>
       </c>
       <c r="AE25" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
@@ -6098,13 +6137,13 @@
         <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="H27" t="s">
         <v>576</v>
       </c>
       <c r="L27" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="Z27" t="s">
         <v>60</v>
@@ -6149,10 +6188,10 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F30" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="H30" t="s">
         <v>578</v>
@@ -6166,7 +6205,7 @@
         <v>484</v>
       </c>
       <c r="F31" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="H31" t="s">
         <v>394</v>
@@ -6177,7 +6216,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="H32" t="s">
         <v>569</v>
@@ -6202,10 +6241,10 @@
         <v>41</v>
       </c>
       <c r="H34" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="Z34" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="35" spans="6:26" x14ac:dyDescent="0.2">
@@ -6271,7 +6310,7 @@
         <v>561</v>
       </c>
       <c r="Z40" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="41" spans="6:26" x14ac:dyDescent="0.2">
@@ -6279,7 +6318,7 @@
         <v>157</v>
       </c>
       <c r="Z41" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="42" spans="6:26" x14ac:dyDescent="0.2">
@@ -6292,7 +6331,7 @@
     </row>
     <row r="43" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H43" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="Z43" t="s">
         <v>69</v>
@@ -6343,7 +6382,7 @@
         <v>209</v>
       </c>
       <c r="Z49" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="50" spans="8:26" x14ac:dyDescent="0.2">
@@ -6367,7 +6406,7 @@
         <v>744</v>
       </c>
       <c r="Z52" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="53" spans="8:26" x14ac:dyDescent="0.2">
@@ -6399,7 +6438,7 @@
         <v>562</v>
       </c>
       <c r="Z56" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="57" spans="8:26" x14ac:dyDescent="0.2">
@@ -6407,7 +6446,7 @@
         <v>586</v>
       </c>
       <c r="Z57" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="58" spans="8:26" x14ac:dyDescent="0.2">
@@ -6420,7 +6459,7 @@
     </row>
     <row r="59" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H59" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="Z59" t="s">
         <v>702</v>
@@ -6431,7 +6470,7 @@
         <v>588</v>
       </c>
       <c r="Z60" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="61" spans="8:26" x14ac:dyDescent="0.2">
@@ -6495,7 +6534,7 @@
         <v>664</v>
       </c>
       <c r="Z68" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="69" spans="8:26" x14ac:dyDescent="0.2">
@@ -6503,7 +6542,7 @@
         <v>608</v>
       </c>
       <c r="Z69" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="70" spans="8:26" x14ac:dyDescent="0.2">
@@ -6516,7 +6555,7 @@
     </row>
     <row r="71" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H71" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="Z71" t="s">
         <v>768</v>
@@ -6527,12 +6566,12 @@
         <v>609</v>
       </c>
       <c r="Z72" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="73" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H73" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="Z73" t="s">
         <v>87</v>
@@ -6548,7 +6587,7 @@
     </row>
     <row r="75" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H75" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="Z75" t="s">
         <v>89</v>
@@ -6564,7 +6603,7 @@
     </row>
     <row r="77" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H77" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="Z77" t="s">
         <v>195</v>
@@ -6583,7 +6622,7 @@
         <v>574</v>
       </c>
       <c r="Z79" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="80" spans="8:26" x14ac:dyDescent="0.2">
@@ -6591,7 +6630,7 @@
         <v>580</v>
       </c>
       <c r="Z80" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="81" spans="8:26" x14ac:dyDescent="0.2">
@@ -6604,7 +6643,7 @@
     </row>
     <row r="82" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H82" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="Z82" t="s">
         <v>92</v>
@@ -6623,7 +6662,7 @@
         <v>564</v>
       </c>
       <c r="Z84" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="85" spans="8:26" x14ac:dyDescent="0.2">
@@ -6652,10 +6691,10 @@
     </row>
     <row r="88" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="Z88" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="89" spans="8:26" x14ac:dyDescent="0.2">
@@ -6671,7 +6710,7 @@
         <v>582</v>
       </c>
       <c r="Z90" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="91" spans="8:26" x14ac:dyDescent="0.2">
@@ -6695,7 +6734,7 @@
         <v>600</v>
       </c>
       <c r="Z93" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="94" spans="8:26" x14ac:dyDescent="0.2">
@@ -6703,7 +6742,7 @@
         <v>606</v>
       </c>
       <c r="Z94" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="95" spans="8:26" x14ac:dyDescent="0.2">
@@ -6735,12 +6774,12 @@
         <v>572</v>
       </c>
       <c r="Z98" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="99" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z99" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="100" spans="8:26" x14ac:dyDescent="0.2">
@@ -6775,17 +6814,17 @@
     </row>
     <row r="106" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z106" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="107" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z107" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="108" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z108" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="109" spans="8:26" x14ac:dyDescent="0.2">
@@ -6795,7 +6834,7 @@
     </row>
     <row r="110" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z110" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="111" spans="8:26" x14ac:dyDescent="0.2">
@@ -6870,7 +6909,7 @@
     </row>
     <row r="125" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z125" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="126" spans="26:26" x14ac:dyDescent="0.2">
@@ -6880,7 +6919,7 @@
     </row>
     <row r="127" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z127" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="128" spans="26:26" x14ac:dyDescent="0.2">
@@ -6969,10 +7008,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -7194,7 +7233,7 @@
     </row>
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="12" t="s">
@@ -7204,10 +7243,10 @@
         <v>168</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>972</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>973</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -7229,10 +7268,10 @@
         <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>973</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>974</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>975</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -7251,13 +7290,13 @@
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -18505,7 +18544,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18539,10 +18578,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -18658,7 +18697,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="24" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="14"/>
@@ -18696,7 +18735,7 @@
     <row r="7" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>13</v>
@@ -18721,7 +18760,7 @@
     <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>13</v>
@@ -18745,10 +18784,10 @@
     </row>
     <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>13</v>
@@ -18777,7 +18816,7 @@
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10" s="57" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>13</v>
@@ -18786,7 +18825,7 @@
         <v>614</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F10"/>
       <c r="G10"/>
@@ -18806,7 +18845,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>279</v>
@@ -18843,7 +18882,7 @@
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13" s="8" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>31</v>
@@ -18852,7 +18891,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>392</v>
@@ -18867,7 +18906,7 @@
     <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>31</v>
@@ -18876,7 +18915,7 @@
         <v>26</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>540</v>
@@ -18891,7 +18930,7 @@
     <row r="15" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15" s="8" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>13</v>
@@ -18900,7 +18939,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -18912,10 +18951,10 @@
     </row>
     <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>13</v>
@@ -18924,7 +18963,7 @@
         <v>43</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -18937,7 +18976,7 @@
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17" s="8" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>13</v>
@@ -18946,18 +18985,18 @@
         <v>542</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>546</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17" s="25" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="K17"/>
       <c r="L17"/>
@@ -18965,7 +19004,7 @@
     <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18" s="8" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>13</v>
@@ -18974,7 +19013,7 @@
         <v>43</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
@@ -18987,13 +19026,13 @@
     <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19" s="8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -19016,7 +19055,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -19029,7 +19068,7 @@
     <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21" s="8" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>13</v>
@@ -19038,7 +19077,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -19051,7 +19090,7 @@
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22" s="8" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>13</v>
@@ -19060,10 +19099,10 @@
         <v>610</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>852</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>853</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>854</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
@@ -19075,7 +19114,7 @@
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>13</v>
@@ -19084,7 +19123,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
@@ -19096,19 +19135,19 @@
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
@@ -19121,7 +19160,7 @@
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>13</v>
@@ -19130,7 +19169,7 @@
         <v>43</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="F25"/>
       <c r="G25"/>
@@ -19150,7 +19189,7 @@
         <v>40</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>279</v>
@@ -19165,7 +19204,7 @@
     <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27" s="8" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>13</v>
@@ -19189,7 +19228,7 @@
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>31</v>
@@ -19198,7 +19237,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>392</v>
@@ -19213,7 +19252,7 @@
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>13</v>
@@ -19222,7 +19261,7 @@
         <v>43</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F29"/>
       <c r="G29"/>
@@ -19235,7 +19274,7 @@
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="8" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>31</v>
@@ -19244,7 +19283,7 @@
         <v>26</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>540</v>
@@ -19259,7 +19298,7 @@
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>13</v>
@@ -19268,7 +19307,7 @@
         <v>43</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F31"/>
       <c r="G31"/>
@@ -19297,7 +19336,7 @@
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1048576" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>target</formula1>
     </dataValidation>
@@ -19312,24 +19351,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="64.33203125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.1640625" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.5" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="54" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="53.5" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="58.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="20.5" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.6640625" style="25" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.83203125" style="25" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="1.6640625" style="10" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" style="15" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="12.5" style="16" customWidth="1" collapsed="1"/>
@@ -19352,10 +19391,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -19452,7 +19491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>629</v>
       </c>
@@ -19479,7 +19518,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="12" t="s">
@@ -19502,7 +19541,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>622</v>
@@ -19529,7 +19568,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>630</v>
@@ -19556,7 +19595,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>631</v>
@@ -19581,7 +19620,7 @@
       <c r="N9" s="14"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>632</v>
@@ -19606,7 +19645,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="27" t="s">
         <v>633</v>
@@ -19633,7 +19672,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>634</v>
@@ -19648,7 +19687,7 @@
         <v>625</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>784</v>
+        <v>1091</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>235</v>
@@ -19662,7 +19701,7 @@
       <c r="N12" s="14"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>628</v>
       </c>
@@ -19687,7 +19726,7 @@
       <c r="N13" s="14"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>623</v>
@@ -19714,7 +19753,7 @@
       <c r="N14" s="14"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
@@ -19737,6 +19776,152 @@
       <c r="N15" s="14"/>
       <c r="O15" s="2"/>
     </row>
+    <row r="16" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -19810,10 +19995,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -19829,7 +20014,7 @@
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -19972,7 +20157,7 @@
         <v>43</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
@@ -20018,7 +20203,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -20148,7 +20333,7 @@
         <v>671</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
@@ -20272,7 +20457,7 @@
         <v>43</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F19" s="40"/>
       <c r="G19" s="37"/>
@@ -20295,7 +20480,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F20" s="40"/>
       <c r="G20" s="37"/>
@@ -20318,7 +20503,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
@@ -20334,7 +20519,7 @@
     <row r="22" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="53"/>
       <c r="B22" s="33" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C22" s="36" t="s">
         <v>183</v>
@@ -20370,7 +20555,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
@@ -20420,7 +20605,7 @@
         <v>43</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="37"/>
@@ -20443,7 +20628,7 @@
         <v>43</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
@@ -20466,7 +20651,7 @@
         <v>43</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
@@ -20491,7 +20676,7 @@
         <v>43</v>
       </c>
       <c r="E28" s="47" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
@@ -20519,7 +20704,7 @@
         <v>714</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>241</v>
@@ -20546,7 +20731,7 @@
         <v>714</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>235</v>
@@ -20677,7 +20862,7 @@
         <v>723</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>235</v>
@@ -20704,7 +20889,7 @@
         <v>723</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G36" s="37" t="s">
         <v>235</v>
@@ -20731,7 +20916,7 @@
         <v>723</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G37" s="37" t="s">
         <v>235</v>
@@ -20758,7 +20943,7 @@
         <v>723</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>235</v>
@@ -20833,7 +21018,7 @@
         <v>725</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G41" s="37"/>
       <c r="H41" s="37"/>
@@ -20870,7 +21055,7 @@
     </row>
     <row r="43" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="53" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B43" s="33"/>
       <c r="C43" s="36" t="s">
@@ -20905,10 +21090,10 @@
         <v>40</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="G44"/>
       <c r="H44"/>
@@ -20927,10 +21112,10 @@
         <v>40</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F45" s="42" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="G45"/>
       <c r="H45"/>
@@ -20946,13 +21131,13 @@
         <v>31</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G46"/>
       <c r="H46"/>
@@ -21035,10 +21220,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -21333,10 +21518,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -21577,7 +21762,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>480</v>
@@ -21647,7 +21832,7 @@
     </row>
     <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="12" t="s">
@@ -21657,14 +21842,14 @@
         <v>43</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="24" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="14"/>
@@ -21682,7 +21867,7 @@
         <v>40</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>235</v>
@@ -21707,14 +21892,14 @@
         <v>43</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="24" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="14"/>
@@ -21732,14 +21917,14 @@
         <v>37</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="24" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="14"/>
@@ -21757,14 +21942,14 @@
         <v>37</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17" s="24" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="K17"/>
       <c r="L17"/>
@@ -21779,14 +21964,14 @@
         <v>37</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18" s="24" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="K18"/>
       <c r="L18"/>
@@ -21798,7 +21983,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>540</v>
@@ -21810,14 +21995,14 @@
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19" s="24" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="K19"/>
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="63" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B20"/>
       <c r="C20" s="13" t="s">
@@ -21827,7 +22012,7 @@
         <v>40</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>241</v>
@@ -21849,7 +22034,7 @@
         <v>40</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>621</v>
@@ -21871,7 +22056,7 @@
         <v>40</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>540</v>
@@ -21886,13 +22071,13 @@
     <row r="23" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="8" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>540</v>
@@ -21911,24 +22096,24 @@
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24" s="13" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>956</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>957</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>958</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24" s="25" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
@@ -21936,13 +22121,13 @@
     <row r="25" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="8" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>540</v>
@@ -21964,7 +22149,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>540</v>
@@ -21983,31 +22168,31 @@
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27" s="13" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27" s="25" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="K27"/>
       <c r="L27"/>
     </row>
     <row r="28" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="63" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B28"/>
       <c r="C28" s="13" t="s">
@@ -22017,10 +22202,10 @@
         <v>40</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
@@ -22046,14 +22231,14 @@
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" s="25" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="K29"/>
       <c r="L29"/>
     </row>
     <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="63" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B30"/>
       <c r="C30" s="13" t="s">
@@ -22063,10 +22248,10 @@
         <v>40</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>1072</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>1073</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
@@ -22085,10 +22270,10 @@
         <v>35</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
@@ -22099,7 +22284,7 @@
     </row>
     <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="63" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B32"/>
       <c r="C32" s="13" t="s">
@@ -22109,7 +22294,7 @@
         <v>40</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>235</v>
@@ -22131,10 +22316,10 @@
         <v>40</v>
       </c>
       <c r="E33" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>1076</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>1077</v>
       </c>
       <c r="G33"/>
       <c r="H33"/>
@@ -22153,7 +22338,7 @@
         <v>43</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F34"/>
       <c r="G34"/>
@@ -22206,9 +22391,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D87D36E-04A6-D640-B45B-3F4AC7187531}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22241,10 +22426,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -22260,7 +22445,7 @@
     </row>
     <row r="2" spans="1:15" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -22343,7 +22528,7 @@
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B5"/>
       <c r="C5" s="13" t="s">
@@ -22356,7 +22541,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -22378,7 +22563,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
@@ -22444,7 +22629,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
@@ -22455,20 +22640,20 @@
     </row>
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B10"/>
       <c r="C10" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>949</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>950</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>951</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -22484,13 +22669,13 @@
         <v>31</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -22504,7 +22689,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>15</v>
@@ -22608,10 +22793,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -22804,7 +22989,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="24" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="14"/>
@@ -23833,7 +24018,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="14"/>
@@ -23862,7 +24047,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="14"/>
@@ -23891,7 +24076,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="14"/>
@@ -23920,7 +24105,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="14"/>
@@ -23945,7 +24130,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="14"/>
@@ -24010,7 +24195,7 @@
     <row r="54" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>13</v>
@@ -24019,7 +24204,7 @@
         <v>43</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -24220,7 +24405,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
       <c r="J62" s="24" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="K62" s="2"/>
       <c r="L62" s="14"/>
@@ -24802,7 +24987,7 @@
     <row r="86" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>13</v>
@@ -24831,7 +25016,7 @@
     <row r="87" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>13</v>
@@ -25061,7 +25246,7 @@
         <v>31</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>481</v>
@@ -25090,7 +25275,7 @@
         <v>31</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>482</v>
@@ -25214,10 +25399,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -25588,10 +25773,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -25690,7 +25875,7 @@
     </row>
     <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
@@ -25700,7 +25885,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -25748,14 +25933,14 @@
         <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="24" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="14"/>
@@ -26328,10 +26513,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -27027,10 +27212,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -27588,7 +27773,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>459</v>
@@ -27613,7 +27798,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>460</v>
@@ -27638,7 +27823,7 @@
         <v>31</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>462</v>
@@ -27663,7 +27848,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>463</v>
@@ -27688,7 +27873,7 @@
         <v>31</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>465</v>
@@ -27713,7 +27898,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>466</v>
@@ -27738,7 +27923,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>467</v>
@@ -27763,7 +27948,7 @@
         <v>31</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>468</v>
@@ -27788,7 +27973,7 @@
         <v>31</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>470</v>
@@ -27813,7 +27998,7 @@
         <v>31</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>471</v>
@@ -27978,10 +28163,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -29161,10 +29346,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -29180,7 +29365,7 @@
     </row>
     <row r="2" spans="1:15" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -29270,7 +29455,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>540</v>
@@ -29389,10 +29574,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>796</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>797</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -29629,7 +29814,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>431</v>

</xml_diff>